<commit_message>
Filled in my execution for the sprint
</commit_message>
<xml_diff>
--- a/sprint_backlog/sprint1/execution.xlsx
+++ b/sprint_backlog/sprint1/execution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammed\Dropbox\UTSC\Third Year\First Semester\CSCC01\Team5\sprint_backlog\sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18278558-F69D-4C5D-8C19-CFD1AF22E27C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D87C6D-219F-4B8A-9135-05B78AABF496}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16386" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <r>
       <rPr>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t xml:space="preserve">Sprint 1 Execution </t>
+  </si>
+  <si>
+    <t>M:1</t>
   </si>
 </sst>
 </file>
@@ -315,6 +318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -324,7 +328,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -723,32 +726,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
@@ -814,7 +817,7 @@
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -833,7 +836,7 @@
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -850,7 +853,7 @@
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="4"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
@@ -886,7 +889,7 @@
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -903,7 +906,7 @@
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
@@ -920,7 +923,7 @@
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -939,7 +942,7 @@
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="4"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="3" t="s">
         <v>28</v>
       </c>
@@ -956,7 +959,7 @@
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -973,7 +976,7 @@
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="3" t="s">
         <v>31</v>
       </c>
@@ -990,7 +993,7 @@
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1000,14 +1003,24 @@
       <c r="D16" s="3">
         <v>5</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="4"/>
+      <c r="A17" s="5"/>
       <c r="B17" s="3" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Fixed up inconsistencies in sprint 1
</commit_message>
<xml_diff>
--- a/sprint_backlog/sprint1/execution.xlsx
+++ b/sprint_backlog/sprint1/execution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ajg\Documents (D)\Repositories\CSCC01\Team5\sprint_backlog\sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF5E904-0333-4A38-8FED-104D24EA08C8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11325FB4-B724-4129-9E29-5C4A3FEAA21D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <r>
       <rPr>
@@ -197,18 +197,9 @@
     <t>Changes in Story Points</t>
   </si>
   <si>
-    <t>T2 took less time than expected and was completed in 2 story points</t>
-  </si>
-  <si>
-    <t>T4 also took less time than expected and was completed in 4 story points</t>
-  </si>
-  <si>
     <t>Due to personal events Saad was unable to start T4 until day 5 so Alex split the task with him</t>
   </si>
   <si>
-    <t>A:2, S:2</t>
-  </si>
-  <si>
     <t>Completed</t>
   </si>
   <si>
@@ -219,6 +210,15 @@
   </si>
   <si>
     <t>W:1</t>
+  </si>
+  <si>
+    <t>A:2</t>
+  </si>
+  <si>
+    <t>T2 took less time than expected and was completed on day 4</t>
+  </si>
+  <si>
+    <t>A:2, S:3</t>
   </si>
 </sst>
 </file>
@@ -250,7 +250,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -366,18 +365,14 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -390,6 +385,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:I14"/>
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,33 +789,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
+      <c r="A1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -846,8 +845,8 @@
       <c r="I3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>50</v>
+      <c r="J3" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -870,8 +869,8 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="10" t="s">
-        <v>51</v>
+      <c r="J4" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -882,8 +881,8 @@
         <v>13</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="8">
-        <v>2</v>
+      <c r="D5" s="14">
+        <v>3</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -891,11 +890,11 @@
         <v>44</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="10" t="s">
-        <v>51</v>
+      <c r="J5" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -916,32 +915,32 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="10"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="8">
-        <v>4</v>
+      <c r="D7" s="14">
+        <v>5</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
@@ -956,7 +955,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="10"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -976,10 +975,10 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="10"/>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="13" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -994,10 +993,10 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="10"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
@@ -1012,10 +1011,10 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="10"/>
+      <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="13" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1032,10 +1031,10 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="10"/>
+      <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="3" t="s">
         <v>28</v>
       </c>
@@ -1050,10 +1049,10 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="10"/>
+      <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="13" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1064,26 +1063,26 @@
         <v>5</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="3" t="s">
         <v>31</v>
       </c>
@@ -1098,10 +1097,10 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="10"/>
+      <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="13" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1127,11 +1126,11 @@
         <v>43</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="3" t="s">
         <v>35</v>
       </c>
@@ -1146,7 +1145,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="10"/>
+      <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -1166,7 +1165,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="10"/>
+      <c r="J18" s="6"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -1186,65 +1185,51 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="10"/>
+      <c r="J19" s="6"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="10">
     <mergeCell ref="A21:I21"/>
     <mergeCell ref="A22:I22"/>
-    <mergeCell ref="A24:I24"/>
     <mergeCell ref="A23:I23"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>

</xml_diff>